<commit_message>
back up manhattan bridge data and NJTPK work
</commit_message>
<xml_diff>
--- a/BEAST/beast_equip/BDI_quote.xlsx
+++ b/BEAST/beast_equip/BDI_quote.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="36" windowWidth="22980" windowHeight="9552" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="36" windowWidth="22980" windowHeight="9552" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="quote1" sheetId="1" r:id="rId1"/>
@@ -580,6 +580,8 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -598,11 +600,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -942,14 +942,14 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="41" t="s">
         <v>50</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="41"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="43"/>
     </row>
     <row r="3" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8">
@@ -1312,14 +1312,14 @@
       </c>
     </row>
     <row r="21" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="42" t="s">
+      <c r="A21" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="B21" s="43"/>
-      <c r="C21" s="43"/>
-      <c r="D21" s="43"/>
-      <c r="E21" s="43"/>
-      <c r="F21" s="44"/>
+      <c r="B21" s="45"/>
+      <c r="C21" s="45"/>
+      <c r="D21" s="45"/>
+      <c r="E21" s="45"/>
+      <c r="F21" s="46"/>
     </row>
     <row r="22" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="8">
@@ -1605,14 +1605,14 @@
       </c>
     </row>
     <row r="36" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="42" t="s">
+      <c r="A36" s="44" t="s">
         <v>52</v>
       </c>
-      <c r="B36" s="43"/>
-      <c r="C36" s="43"/>
-      <c r="D36" s="43"/>
-      <c r="E36" s="43"/>
-      <c r="F36" s="44"/>
+      <c r="B36" s="45"/>
+      <c r="C36" s="45"/>
+      <c r="D36" s="45"/>
+      <c r="E36" s="45"/>
+      <c r="F36" s="46"/>
     </row>
     <row r="37" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="8">
@@ -1691,14 +1691,14 @@
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A41" s="39" t="s">
+      <c r="A41" s="41" t="s">
         <v>62</v>
       </c>
-      <c r="B41" s="40"/>
-      <c r="C41" s="40"/>
-      <c r="D41" s="40"/>
-      <c r="E41" s="40"/>
-      <c r="F41" s="41"/>
+      <c r="B41" s="42"/>
+      <c r="C41" s="42"/>
+      <c r="D41" s="42"/>
+      <c r="E41" s="42"/>
+      <c r="F41" s="43"/>
     </row>
     <row r="42" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="9"/>
@@ -1830,8 +1830,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1869,14 +1869,14 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="41" t="s">
         <v>50</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="41"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="43"/>
     </row>
     <row r="3" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8">
@@ -1934,11 +1934,11 @@
         <v>69.75</v>
       </c>
       <c r="E5" s="5">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F5" s="14">
         <f t="shared" si="0"/>
-        <v>558</v>
+        <v>418.5</v>
       </c>
     </row>
     <row r="6" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -2100,13 +2100,15 @@
       <c r="C13" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="D13" s="23"/>
+      <c r="D13" s="23">
+        <v>225</v>
+      </c>
       <c r="E13" s="22">
         <v>1</v>
       </c>
       <c r="F13" s="24">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>225</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -2268,14 +2270,14 @@
       </c>
     </row>
     <row r="22" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="42" t="s">
+      <c r="A22" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="B22" s="43"/>
-      <c r="C22" s="43"/>
-      <c r="D22" s="43"/>
-      <c r="E22" s="43"/>
-      <c r="F22" s="44"/>
+      <c r="B22" s="45"/>
+      <c r="C22" s="45"/>
+      <c r="D22" s="45"/>
+      <c r="E22" s="45"/>
+      <c r="F22" s="46"/>
     </row>
     <row r="23" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="8">
@@ -2583,14 +2585,14 @@
       </c>
     </row>
     <row r="37" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="42" t="s">
+      <c r="A37" s="44" t="s">
         <v>52</v>
       </c>
-      <c r="B37" s="43"/>
-      <c r="C37" s="43"/>
-      <c r="D37" s="43"/>
-      <c r="E37" s="43"/>
-      <c r="F37" s="44"/>
+      <c r="B37" s="45"/>
+      <c r="C37" s="45"/>
+      <c r="D37" s="45"/>
+      <c r="E37" s="45"/>
+      <c r="F37" s="46"/>
     </row>
     <row r="38" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="8">
@@ -2669,14 +2671,14 @@
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A42" s="39" t="s">
+      <c r="A42" s="41" t="s">
         <v>62</v>
       </c>
-      <c r="B42" s="40"/>
-      <c r="C42" s="40"/>
-      <c r="D42" s="40"/>
-      <c r="E42" s="40"/>
-      <c r="F42" s="41"/>
+      <c r="B42" s="42"/>
+      <c r="C42" s="42"/>
+      <c r="D42" s="42"/>
+      <c r="E42" s="42"/>
+      <c r="F42" s="43"/>
     </row>
     <row r="43" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="9"/>
@@ -2688,11 +2690,11 @@
       <c r="E43" s="6"/>
       <c r="F43" s="20">
         <f>SUM(F3:F9)</f>
-        <v>3639</v>
+        <v>3499.5</v>
       </c>
       <c r="G43" s="38">
         <f>F43/$F$49</f>
-        <v>6.9897859615748084E-2</v>
+        <v>6.7108135089951171E-2</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
@@ -2705,11 +2707,11 @@
       <c r="E44" s="7"/>
       <c r="F44" s="15">
         <f>SUM(F10:F19)</f>
-        <v>8106</v>
+        <v>8331</v>
       </c>
       <c r="G44" s="28">
         <f t="shared" ref="G44:G48" si="3">F44/$F$49</f>
-        <v>0.15569993131224347</v>
+        <v>0.15975935803239982</v>
       </c>
     </row>
     <row r="45" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -2726,7 +2728,7 @@
       </c>
       <c r="G45" s="38">
         <f t="shared" si="3"/>
-        <v>8.7003723275929618E-2</v>
+        <v>8.6861072832701586E-2</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.3">
@@ -2743,7 +2745,7 @@
       </c>
       <c r="G46" s="28">
         <f t="shared" si="3"/>
-        <v>0.49604622824311473</v>
+        <v>0.49523291575881956</v>
       </c>
     </row>
     <row r="47" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -2760,7 +2762,7 @@
       </c>
       <c r="G47" s="38">
         <f t="shared" si="3"/>
-        <v>0.12124311009556357</v>
+        <v>0.12104432109272256</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.3">
@@ -2777,7 +2779,7 @@
       </c>
       <c r="G48" s="28">
         <f t="shared" si="3"/>
-        <v>7.0109147457400531E-2</v>
+        <v>6.9994197193405286E-2</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2790,7 +2792,7 @@
       <c r="E49" s="35"/>
       <c r="F49" s="37">
         <f>SUM(F43:F48)</f>
-        <v>52061.68</v>
+        <v>52147.18</v>
       </c>
     </row>
   </sheetData>
@@ -2808,8 +2810,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H29" sqref="H28:I29"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2841,14 +2843,14 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="46" t="str">
+      <c r="A2" s="47" t="str">
         <f>option1!A2</f>
         <v>DAQ System</v>
       </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
@@ -2864,16 +2866,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="45" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="45">
+    <row r="4" spans="1:5" s="39" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="39">
         <f>option1!A4</f>
         <v>11</v>
       </c>
-      <c r="C4" s="45" t="str">
+      <c r="C4" s="39" t="str">
         <f>option1!C4</f>
         <v>power supply and regulator</v>
       </c>
-      <c r="D4" s="45">
+      <c r="D4" s="39">
         <f>option1!E4</f>
         <v>0</v>
       </c>
@@ -2889,7 +2891,7 @@
       </c>
       <c r="D5">
         <f>option1!E5</f>
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -2906,16 +2908,16 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="45" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="45">
+    <row r="7" spans="1:5" s="39" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="39">
         <f>option1!A7</f>
         <v>14</v>
       </c>
-      <c r="C7" s="45" t="str">
+      <c r="C7" s="39" t="str">
         <f>option1!C7</f>
         <v>12V battery</v>
       </c>
-      <c r="D7" s="45">
+      <c r="D7" s="39">
         <f>option1!E7</f>
         <v>0</v>
       </c>
@@ -2948,61 +2950,61 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="45" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="45">
+    <row r="10" spans="1:5" s="39" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="39">
         <f>option1!A10</f>
         <v>1</v>
       </c>
-      <c r="B10" s="45" t="str">
+      <c r="B10" s="39" t="str">
         <f>option1!B10</f>
         <v>CSI-CR310</v>
       </c>
-      <c r="C10" s="45" t="str">
+      <c r="C10" s="39" t="str">
         <f>option1!C10</f>
         <v>Small Data Logger for sampling analog sensors (hygrometers)</v>
       </c>
-      <c r="D10" s="45">
+      <c r="D10" s="39">
         <f>option1!E10</f>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="45" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="45">
+    <row r="11" spans="1:5" s="39" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="39">
         <f>option1!A11</f>
         <v>2</v>
       </c>
-      <c r="B11" s="45" t="str">
+      <c r="B11" s="39" t="str">
         <f>option1!B11</f>
         <v>CSI-AM16/32</v>
       </c>
-      <c r="C11" s="45" t="str">
+      <c r="C11" s="39" t="str">
         <f>option1!C11</f>
         <v>Multiplexer</v>
       </c>
-      <c r="D11" s="45">
+      <c r="D11" s="39">
         <f>option1!E11</f>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="45" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="45">
+    <row r="12" spans="1:5" s="39" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="39">
         <f>option1!A12</f>
         <v>3</v>
       </c>
-      <c r="B12" s="45" t="str">
+      <c r="B12" s="39" t="str">
         <f>option1!B12</f>
         <v>CSI-19237</v>
       </c>
-      <c r="C12" s="45" t="str">
+      <c r="C12" s="39" t="str">
         <f>option1!C12</f>
         <v>Multiplexer cover</v>
       </c>
-      <c r="D12" s="45">
+      <c r="D12" s="39">
         <f>option1!E12</f>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="45" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" s="39" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>84</v>
       </c>
@@ -3018,23 +3020,23 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="47" t="str">
+      <c r="A14" s="40" t="str">
         <f>option1!A13</f>
         <v>new</v>
       </c>
-      <c r="B14" s="47" t="str">
+      <c r="B14" s="40" t="str">
         <f>option1!B13</f>
         <v>CSI-NL121</v>
       </c>
-      <c r="C14" s="47" t="str">
+      <c r="C14" s="40" t="str">
         <f>option1!C13</f>
         <v>Ethernet interface for CR1000</v>
       </c>
-      <c r="D14" s="47">
+      <c r="D14" s="40">
         <f>option1!E13</f>
         <v>1</v>
       </c>
-      <c r="E14" s="47">
+      <c r="E14" s="40">
         <v>1</v>
       </c>
     </row>
@@ -3163,29 +3165,29 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="46" t="str">
+      <c r="A23" s="47" t="str">
         <f>option1!A22</f>
         <v>Sensors</v>
       </c>
-      <c r="B23" s="46"/>
-      <c r="C23" s="46"/>
-      <c r="D23" s="46"/>
-      <c r="E23" s="46"/>
-    </row>
-    <row r="24" spans="1:5" s="45" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="45">
+      <c r="B23" s="47"/>
+      <c r="C23" s="47"/>
+      <c r="D23" s="47"/>
+      <c r="E23" s="47"/>
+    </row>
+    <row r="24" spans="1:5" s="39" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="39">
         <f>option1!A23</f>
         <v>19</v>
       </c>
-      <c r="B24" s="45" t="str">
+      <c r="B24" s="39" t="str">
         <f>option1!B23</f>
         <v>VW-4000A-2</v>
       </c>
-      <c r="C24" s="45" t="str">
+      <c r="C24" s="39" t="str">
         <f>option1!C23</f>
         <v xml:space="preserve">6" VW gauge </v>
       </c>
-      <c r="D24" s="45">
+      <c r="D24" s="39">
         <f>option1!E23</f>
         <v>0</v>
       </c>
@@ -3194,16 +3196,16 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:5" s="45" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="45">
+    <row r="25" spans="1:5" s="39" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="39">
         <f>option1!A24</f>
         <v>20</v>
       </c>
-      <c r="C25" s="45" t="str">
+      <c r="C25" s="39" t="str">
         <f>option1!C24</f>
         <v>cable for 6" gauges</v>
       </c>
-      <c r="D25" s="45">
+      <c r="D25" s="39">
         <f>option1!E24</f>
         <v>0</v>
       </c>
@@ -3411,14 +3413,14 @@
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A38" s="46" t="str">
+      <c r="A38" s="47" t="str">
         <f>option1!A37</f>
         <v>Miscellaneous</v>
       </c>
-      <c r="B38" s="46"/>
-      <c r="C38" s="46"/>
-      <c r="D38" s="46"/>
-      <c r="E38" s="46"/>
+      <c r="B38" s="47"/>
+      <c r="C38" s="47"/>
+      <c r="D38" s="47"/>
+      <c r="E38" s="47"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39">

</xml_diff>